<commit_message>
changes to the Excel file
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/excelsuites/AdminMatrix.xlsx
+++ b/src/main/java/utilities/excelsuites/AdminMatrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>nombre de la plataforma</t>
   </si>
@@ -49,53 +49,64 @@
     <t>Nombre del Tc</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Oscar1</t>
-  </si>
-  <si>
-    <t>Oscar2</t>
-  </si>
-  <si>
-    <t>Oscar3</t>
-  </si>
-  <si>
-    <t>Oscar4</t>
-  </si>
-  <si>
-    <t>Oscar5</t>
-  </si>
-  <si>
-    <t>Oscar6</t>
-  </si>
-  <si>
-    <t>Oscar7</t>
-  </si>
-  <si>
-    <t>Oscar8</t>
-  </si>
-  <si>
-    <t>Oscar9</t>
-  </si>
-  <si>
-    <t>Oscar10</t>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Actual result</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Log In as Admin</t>
+  </si>
+  <si>
+    <t>Type Authoriacion code</t>
+  </si>
+  <si>
+    <t>Authotizarion code should be entered</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test.admin@ur.com</t>
+  </si>
+  <si>
+    <t>Type user name into the UserName text field</t>
+  </si>
+  <si>
+    <t>User name should be introduces</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,13 +129,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -431,9 +445,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -441,7 +457,7 @@
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,14 +467,8 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -468,28 +478,16 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -499,49 +497,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
         <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Reading test case steps method
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/excelsuites/AdminMatrix.xlsx
+++ b/src/main/java/utilities/excelsuites/AdminMatrix.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19423"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Documents\Eclipse\RouseServicesWindowsVersion\RSProyectwithIntellij\src\main\java\utilities\excelsuites\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06F24B66-FF5C-49D5-A797-078D6689C720}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="TC001" sheetId="2" r:id="rId2"/>
     <sheet name="TC002" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179016"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,62 +27,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>nombre de la plataforma</t>
   </si>
   <si>
+    <t>Nombre del Tc</t>
+  </si>
+  <si>
+    <t>Excel Suite Name</t>
+  </si>
+  <si>
+    <t>SheetName</t>
+  </si>
+  <si>
     <t>Android</t>
   </si>
   <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>AdminMatrix.xlsx</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
     <t>iOS</t>
   </si>
   <si>
-    <t>SheetName</t>
-  </si>
-  <si>
-    <t>TC001</t>
+    <t>Logout</t>
   </si>
   <si>
     <t>TC002</t>
   </si>
   <si>
-    <t>Nombre del Tc</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>Test Case Name</t>
   </si>
   <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Actual result</t>
+  </si>
+  <si>
     <t>Expected result</t>
   </si>
   <si>
-    <t>Actual result</t>
-  </si>
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
     <t>Log In as Admin</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>Type Authoriacion code</t>
   </si>
   <si>
     <t>Authotizarion code should be entered</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>test.admin@ur.com</t>
   </si>
   <si>
@@ -89,19 +96,13 @@
   </si>
   <si>
     <t>User name should be introduces</t>
-  </si>
-  <si>
-    <t>Excel Suite Name</t>
-  </si>
-  <si>
-    <t>AdminMatrix.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,7 +173,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -450,60 +451,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -512,14 +513,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
@@ -529,123 +530,126 @@
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
now the framework is able to click in a button
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/excelsuites/AdminMatrix.xlsx
+++ b/src/main/java/utilities/excelsuites/AdminMatrix.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19423"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20230"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Documents\Eclipse\RouseServicesWindowsVersion\RSProyectwithIntellij\src\main\java\utilities\excelsuites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06F24B66-FF5C-49D5-A797-078D6689C720}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C11FC113-0FF3-4183-8AAD-F4B6A3CB2423}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="TC001" sheetId="2" r:id="rId2"/>
-    <sheet name="TC002" sheetId="3" r:id="rId3"/>
+    <sheet name="TC001-A" sheetId="2" r:id="rId2"/>
+    <sheet name="TC002-i" sheetId="3" r:id="rId3"/>
+    <sheet name="Matrix Sample" sheetId="4" r:id="rId4"/>
+    <sheet name="Test Case Sample structure" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179016"/>
   <extLst>
@@ -27,12 +29,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
-  <si>
-    <t>nombre de la plataforma</t>
-  </si>
-  <si>
-    <t>Nombre del Tc</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>AdminMatrix</t>
+  </si>
+  <si>
+    <t>TC001-A</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>TC002-i</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Allow</t>
+  </si>
+  <si>
+    <t>Type Authoriacion code</t>
+  </si>
+  <si>
+    <t>SendText</t>
+  </si>
+  <si>
+    <t>Xpath</t>
+  </si>
+  <si>
+    <t>test.admin@ur.com</t>
+  </si>
+  <si>
+    <t>Type user name into the UserName text field</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Platform Name</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
   </si>
   <si>
     <t>Excel Suite Name</t>
@@ -44,58 +91,19 @@
     <t>Android</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>AdminMatrix.xlsx</t>
   </si>
   <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>iOS</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Test Case Name</t>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Object</t>
   </si>
   <si>
     <t>Parameter</t>
   </si>
   <si>
     <t>Actual result</t>
-  </si>
-  <si>
-    <t>Expected result</t>
-  </si>
-  <si>
-    <t>Log In as Admin</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Type Authoriacion code</t>
-  </si>
-  <si>
-    <t>Authotizarion code should be entered</t>
-  </si>
-  <si>
-    <t>test.admin@ur.com</t>
-  </si>
-  <si>
-    <t>Type user name into the UserName text field</t>
-  </si>
-  <si>
-    <t>User name should be introduces</t>
   </si>
 </sst>
 </file>
@@ -452,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -481,30 +489,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -514,76 +508,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -591,66 +559,156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B83D68-EE84-485B-BB20-554F491FD68A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" xr3:uid="{0C52F37C-4ABD-5838-B460-8D0F68110DA7}"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4D8C04-19EC-47C2-A5C7-EC84A0497F3C}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" xr3:uid="{3956F413-77A5-5E64-BDB4-36A42CC49129}"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uploading the last changes i modified to the repository
</commit_message>
<xml_diff>
--- a/src/main/java/utilities/excelsuites/AdminMatrix.xlsx
+++ b/src/main/java/utilities/excelsuites/AdminMatrix.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20304"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Documents\Eclipse\RouseServicesWindowsVersion\RSProyectwithIntellij\src\main\java\utilities\excelsuites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9581BCC2-9562-43FB-85F4-E09757ABC44D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAE351E3-A743-4B98-ACD9-FE64C046F169}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="TC001-A" sheetId="2" r:id="rId2"/>
+    <sheet name="TC001-A" sheetId="6" r:id="rId2"/>
     <sheet name="TC002-i" sheetId="3" r:id="rId3"/>
     <sheet name="Matrix Sample" sheetId="4" r:id="rId4"/>
     <sheet name="Test Case Sample structure" sheetId="5" r:id="rId5"/>
@@ -29,20 +29,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>AdminMatrix</t>
+  </si>
+  <si>
+    <t>TC001-A</t>
+  </si>
   <si>
     <t>iOS</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>AdminMatrix</t>
-  </si>
-  <si>
-    <t>TC001-A</t>
-  </si>
-  <si>
     <t>Logout</t>
   </si>
   <si>
@@ -55,42 +58,57 @@
     <t>Id</t>
   </si>
   <si>
+    <t>et_auth_code</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Click in the Continue button</t>
+  </si>
+  <si>
+    <t>SendText</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Send keys to auth code text field</t>
+  </si>
+  <si>
     <t>Allow</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Click in the Continue button</t>
-  </si>
-  <si>
-    <t>SendText</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>//XCUIElementTypeTextField</t>
+  </si>
+  <si>
+    <t>Tap on auth code field</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Type authentication code into the text field</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>Click in the continue button</t>
   </si>
   <si>
     <t>Xpath</t>
   </si>
   <si>
-    <t>//XCUIElementTypeTextField</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Type authentication code into the text field</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Continue</t>
-  </si>
-  <si>
-    <t>Click in the continue button</t>
-  </si>
-  <si>
     <t>//XCUIElementTypeTextField[contains(@value, "Username")]</t>
   </si>
   <si>
+    <t>Tap on username text field</t>
+  </si>
+  <si>
     <t>test.admin@ur.com</t>
   </si>
   <si>
@@ -100,6 +118,9 @@
     <t>//XCUIElementTypeSecureTextField[contains(@value, Password)]</t>
   </si>
   <si>
+    <t>Tap on password text field</t>
+  </si>
+  <si>
     <t>Type password</t>
   </si>
   <si>
@@ -109,12 +130,6 @@
     <t>Click in the Log in button</t>
   </si>
   <si>
-    <t>Type Authoriacion code</t>
-  </si>
-  <si>
-    <t>Type user name into the UserName text field</t>
-  </si>
-  <si>
     <t>Platform Name</t>
   </si>
   <si>
@@ -125,9 +140,6 @@
   </si>
   <si>
     <t>SheetName</t>
-  </si>
-  <si>
-    <t>Android</t>
   </si>
   <si>
     <t>AdminMatrix.xlsx</t>
@@ -504,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -513,6 +525,7 @@
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -531,16 +544,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -549,136 +562,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF1C6AC9-9306-46D0-B74E-19164586032E}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0" xr3:uid="{4E9DD3EA-81F7-5097-9588-5D4AFDBD3AEC}">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{FA68F7E2-3A61-4CD1-9E53-6F66B1A9CDE6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -686,35 +623,163 @@
     <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{905FA56C-1D62-4F1C-B594-63CEE9B86C3A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -729,27 +794,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -757,16 +822,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -786,67 +851,67 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>